<commit_message>
updated CSV files for 30/70 split w/ and w/o punctuation
</commit_message>
<xml_diff>
--- a/NLTK Sentanal/Data/sentanalResults(30-70).xlsx
+++ b/NLTK Sentanal/Data/sentanalResults(30-70).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Desktop\SW Development\Sentanal\NLTK Sentanal\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EEE724E-67B5-46B7-844C-7822DE6816FF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4579F075-B6FE-409A-AAA8-321823C96DDA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,8 +17,6 @@
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">sentanalResults!$A$2:$A$1002</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">sentanalResults!$A$2:$A$1002</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">sentanalResults!$A$2:$A$1002</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
   <si>
     <t>Accuracy</t>
   </si>
@@ -59,7 +57,16 @@
     <t>Split: 30/70</t>
   </si>
   <si>
-    <t>Average Accuracy</t>
+    <t>AVG:</t>
+  </si>
+  <si>
+    <t>MAX:</t>
+  </si>
+  <si>
+    <t>MIN:</t>
+  </si>
+  <si>
+    <t>NO PUNCT</t>
   </si>
 </sst>
 </file>
@@ -383,7 +390,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -498,6 +505,131 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -543,8 +675,17 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1307,16 +1448,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>4762</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>14288</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>309562</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>42863</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -1352,7 +1493,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="8772525" y="180975"/>
+              <a:off x="5805487" y="1295401"/>
               <a:ext cx="4572000" cy="2743200"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -1683,10 +1824,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I1002"/>
+  <dimension ref="A1:P1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="Q22" sqref="Q22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1694,9 +1835,10 @@
     <col min="2" max="2" width="13.59765625" customWidth="1"/>
     <col min="3" max="3" width="13.19921875" customWidth="1"/>
     <col min="9" max="9" width="14.3984375" customWidth="1"/>
+    <col min="16" max="16" width="10.06640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1718,11 +1860,11 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2">
         <v>0.71186440699999998</v>
       </c>
@@ -1744,11 +1886,32 @@
       <c r="G2">
         <v>0.58241758200000004</v>
       </c>
-      <c r="I2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="I2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="P2" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>0.74011299435028199</v>
       </c>
@@ -1770,12 +1933,39 @@
       <c r="G3">
         <v>0.659340659340659</v>
       </c>
-      <c r="I3">
-        <f>AVERAGE(A2:A1002)</f>
+      <c r="I3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="5">
+        <f>AVERAGE(A:A)</f>
         <v>0.72276875666728124</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K3" s="5">
+        <f t="shared" ref="K3:P3" si="0">AVERAGE(B:B)</f>
+        <v>0.75264094994172603</v>
+      </c>
+      <c r="L3" s="5">
+        <f t="shared" si="0"/>
+        <v>0.68315428750199447</v>
+      </c>
+      <c r="M3" s="5">
+        <f t="shared" si="0"/>
+        <v>0.66682309747009483</v>
+      </c>
+      <c r="N3" s="5">
+        <f t="shared" si="0"/>
+        <v>0.82459086541246907</v>
+      </c>
+      <c r="O3" s="5">
+        <f t="shared" si="0"/>
+        <v>0.86645912227278477</v>
+      </c>
+      <c r="P3" s="5">
+        <f t="shared" si="0"/>
+        <v>0.58697346609392909</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>0.71751412429378503</v>
       </c>
@@ -1797,8 +1987,39 @@
       <c r="G4">
         <v>0.61538461538461497</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="I4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="1">
+        <f>MAX(A:A)</f>
+        <v>0.81920903954802204</v>
+      </c>
+      <c r="K4" s="1">
+        <f t="shared" ref="K4:P4" si="1">MAX(B:B)</f>
+        <v>0.82795698924731098</v>
+      </c>
+      <c r="L4" s="1">
+        <f t="shared" si="1"/>
+        <v>0.81111111111111101</v>
+      </c>
+      <c r="M4" s="1">
+        <f t="shared" si="1"/>
+        <v>0.79545454545454497</v>
+      </c>
+      <c r="N4" s="1">
+        <f t="shared" si="1"/>
+        <v>0.97916666666666596</v>
+      </c>
+      <c r="O4" s="1">
+        <f t="shared" si="1"/>
+        <v>0.98837209302325502</v>
+      </c>
+      <c r="P4" s="1">
+        <f t="shared" si="1"/>
+        <v>0.80219780219780201</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5">
         <v>0.71186440677966101</v>
       </c>
@@ -1820,11 +2041,39 @@
       <c r="G5">
         <v>0.59340659340659296</v>
       </c>
-      <c r="I5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="I5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="1">
+        <f>MIN(A:A)</f>
+        <v>0.62711864406779605</v>
+      </c>
+      <c r="K5" s="1">
+        <f t="shared" ref="K5:P5" si="2">MIN(B:B)</f>
+        <v>0.69158878504672805</v>
+      </c>
+      <c r="L5" s="1">
+        <f t="shared" si="2"/>
+        <v>0.52857142857142803</v>
+      </c>
+      <c r="M5" s="1">
+        <f t="shared" si="2"/>
+        <v>0.578125</v>
+      </c>
+      <c r="N5" s="1">
+        <f t="shared" si="2"/>
+        <v>0.73333333333333295</v>
+      </c>
+      <c r="O5" s="1">
+        <f t="shared" si="2"/>
+        <v>0.72093023255813904</v>
+      </c>
+      <c r="P5" s="1">
+        <f t="shared" si="2"/>
+        <v>0.40659340659340598</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>0.62711864406779605</v>
       </c>
@@ -1846,12 +2095,8 @@
       <c r="G6">
         <v>0.40659340659340598</v>
       </c>
-      <c r="I6">
-        <f>AVERAGE(B2:B1002)</f>
-        <v>0.75264094994172603</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>0.72881355932203296</v>
       </c>
@@ -1874,7 +2119,7 @@
         <v>0.52747252747252704</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>0.73446327683615797</v>
       </c>
@@ -1896,11 +2141,8 @@
       <c r="G8">
         <v>0.659340659340659</v>
       </c>
-      <c r="I8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>0.72881355932203296</v>
       </c>
@@ -1922,12 +2164,8 @@
       <c r="G9">
         <v>0.61538461538461497</v>
       </c>
-      <c r="I9">
-        <f>AVERAGE(C2:C1002)</f>
-        <v>0.68315428750199447</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>0.75706214689265505</v>
       </c>
@@ -1950,7 +2188,7 @@
         <v>0.64835164835164805</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>0.70621468926553599</v>
       </c>
@@ -1972,11 +2210,8 @@
       <c r="G11">
         <v>0.60439560439560402</v>
       </c>
-      <c r="I11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>0.70621468926553599</v>
       </c>
@@ -1998,12 +2233,8 @@
       <c r="G12">
         <v>0.59340659340659296</v>
       </c>
-      <c r="I12">
-        <f>AVERAGE(D2:D1002)</f>
-        <v>0.66682309747009483</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>0.74011299435028199</v>
       </c>
@@ -2026,7 +2257,7 @@
         <v>0.62637362637362604</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>0.71186440677966101</v>
       </c>
@@ -2048,11 +2279,8 @@
       <c r="G14">
         <v>0.53846153846153799</v>
       </c>
-      <c r="I14" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>0.75141242937853103</v>
       </c>
@@ -2074,12 +2302,8 @@
       <c r="G15">
         <v>0.67032967032966995</v>
       </c>
-      <c r="I15">
-        <f>AVERAGE(E2:E1002)</f>
-        <v>0.82459086541246907</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>0.74576271186440601</v>
       </c>
@@ -2102,7 +2326,7 @@
         <v>0.63736263736263699</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>0.71751412429378503</v>
       </c>
@@ -2124,11 +2348,8 @@
       <c r="G17">
         <v>0.59340659340659296</v>
       </c>
-      <c r="I17" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>0.73446327683615797</v>
       </c>
@@ -2150,12 +2371,8 @@
       <c r="G18">
         <v>0.59340659340659296</v>
       </c>
-      <c r="I18">
-        <f>AVERAGE(F2:F1002)</f>
-        <v>0.86645912227278477</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>0.76836158192090398</v>
       </c>
@@ -2178,7 +2395,7 @@
         <v>0.71428571428571397</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>0.70621468926553599</v>
       </c>
@@ -2200,11 +2417,8 @@
       <c r="G20">
         <v>0.57142857142857095</v>
       </c>
-      <c r="I20" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>0.71186440677966101</v>
       </c>
@@ -2226,12 +2440,8 @@
       <c r="G21">
         <v>0.57142857142857095</v>
       </c>
-      <c r="I21">
-        <f>AVERAGE(G2:G1002)</f>
-        <v>0.58697346609392909</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>0.76836158192090398</v>
       </c>
@@ -2254,7 +2464,7 @@
         <v>0.659340659340659</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>0.67231638418079098</v>
       </c>
@@ -2277,7 +2487,7 @@
         <v>0.54945054945054905</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>0.70621468926553599</v>
       </c>
@@ -2300,7 +2510,7 @@
         <v>0.56043956043956</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>0.73446327683615797</v>
       </c>
@@ -2323,7 +2533,7 @@
         <v>0.61538461538461497</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>0.69491525423728795</v>
       </c>
@@ -2346,7 +2556,7 @@
         <v>0.58241758241758201</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>0.74011299435028199</v>
       </c>
@@ -2369,7 +2579,7 @@
         <v>0.62637362637362604</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>0.72881355932203296</v>
       </c>
@@ -2392,7 +2602,7 @@
         <v>0.54945054945054905</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>0.72881355932203296</v>
       </c>
@@ -2415,7 +2625,7 @@
         <v>0.67032967032966995</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>0.72316384180790905</v>
       </c>
@@ -2438,7 +2648,7 @@
         <v>0.58241758241758201</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>0.72881355932203296</v>
       </c>
@@ -2461,7 +2671,7 @@
         <v>0.67032967032966995</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>0.75706214689265505</v>
       </c>

</xml_diff>

<commit_message>
testing at 80-20 split and upgraded some files
</commit_message>
<xml_diff>
--- a/NLTK Sentanal/Data/sentanalResults(30-70).xlsx
+++ b/NLTK Sentanal/Data/sentanalResults(30-70).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Desktop\SW Development\Sentanal\NLTK Sentanal\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4579F075-B6FE-409A-AAA8-321823C96DDA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D54C42E-5A82-4CBB-B31C-1062A7980F5A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,6 +17,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">sentanalResults!$A$2:$A$1002</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">sentanalResults!$A$2:$A$1002</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -733,6 +734,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF207ED4"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -756,31 +762,45 @@
   <cx:chart>
     <cx:title pos="t" align="ctr" overlay="0">
       <cx:tx>
-        <cx:txData>
-          <cx:v>30/70 Split Accuracy Histogram</cx:v>
-        </cx:txData>
+        <cx:rich>
+          <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr" rtl="0">
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+              </a:rPr>
+              <a:t>30/70 Split Accuracy Histogram</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr algn="ctr" rtl="0">
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+              </a:rPr>
+              <a:t>(graphed for 1000 runs)</a:t>
+            </a:r>
+          </a:p>
+        </cx:rich>
       </cx:tx>
-      <cx:txPr>
-        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr" rtl="0">
-            <a:defRPr/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:sysClr>
-              </a:solidFill>
-              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-            </a:rPr>
-            <a:t>30/70 Split Accuracy Histogram</a:t>
-          </a:r>
-        </a:p>
-      </cx:txPr>
     </cx:title>
     <cx:plotArea>
       <cx:plotAreaRegion>
@@ -796,14 +816,15 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr algn="ctr" rtl="0">
-                  <a:defRPr/>
+                  <a:defRPr>
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:defRPr>
                 </a:pPr>
                 <a:endParaRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
-                    <a:sysClr val="windowText" lastClr="000000">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:sysClr>
+                    <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:latin typeface="Calibri" panose="020F0502020204030204"/>
                 </a:endParaRPr>
@@ -849,7 +870,7 @@
           </cx:txPr>
         </cx:title>
         <cx:tickLabels/>
-        <cx:numFmt formatCode="0.000" sourceLinked="0"/>
+        <cx:numFmt formatCode="0.00" sourceLinked="0"/>
       </cx:axis>
       <cx:axis id="1">
         <cx:valScaling/>
@@ -892,6 +913,15 @@
         <a:schemeClr val="tx1"/>
       </a:solidFill>
     </a:ln>
+    <a:effectLst>
+      <a:glow rad="63500">
+        <a:schemeClr val="accent6">
+          <a:satMod val="175000"/>
+          <a:alpha val="40000"/>
+        </a:schemeClr>
+      </a:glow>
+      <a:softEdge rad="0"/>
+    </a:effectLst>
   </cx:spPr>
 </cx:chartSpace>
 </file>
@@ -1449,15 +1479,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>4762</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>14288</xdr:rowOff>
+      <xdr:colOff>4761</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>176211</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>309562</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>42863</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>585787</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -1493,8 +1523,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="5805487" y="1295401"/>
-              <a:ext cx="4572000" cy="2743200"/>
+              <a:off x="5805486" y="1095374"/>
+              <a:ext cx="7186614" cy="4276726"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1826,15 +1856,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+    <sheetView tabSelected="1" topLeftCell="D3" workbookViewId="0">
+      <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="13.59765625" customWidth="1"/>
     <col min="3" max="3" width="13.19921875" customWidth="1"/>
-    <col min="9" max="9" width="14.3984375" customWidth="1"/>
+    <col min="9" max="9" width="9.86328125" customWidth="1"/>
     <col min="16" max="16" width="10.06640625" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>